<commit_message>
Update performance dashboard 2026-01-09 17:52 - Simplified Design v3.1
</commit_message>
<xml_diff>
--- a/performance-dashboard/archive/Trading_Performance_20260109.xlsx
+++ b/performance-dashboard/archive/Trading_Performance_20260109.xlsx
@@ -536,26 +536,26 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>¥1,012,068.30</t>
+          <t>¥1,019,638.10</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>¥+12,068.30</t>
+          <t>¥+19,638.10</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>+1.21%</t>
+          <t>+1.96%</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+22.33%</t>
+          <t>+35.84%</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>3.13</v>
+        <v>4.648</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -564,24 +564,24 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>71.4%</t>
+          <t>73.3%</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.0865%</t>
+          <t>0.1306%</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>6.3329%</t>
+          <t>6.6552%</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -590,7 +590,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -612,26 +612,26 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>¥1,034,427.67</t>
+          <t>¥1,042,439.98</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>¥+34,427.67</t>
+          <t>¥+42,439.98</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>+3.44%</t>
+          <t>+4.24%</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+76.59%</t>
+          <t>+92.44%</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>5.698</v>
+        <v>6.638</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -640,24 +640,24 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>64.3%</t>
+          <t>66.7%</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.2442%</t>
+          <t>0.2796%</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>10.4544%</t>
+          <t>10.3159%</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -666,7 +666,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -688,26 +688,26 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>¥1,008,252.47</t>
+          <t>¥1,014,809.18</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>¥+8,252.47</t>
+          <t>¥+14,809.18</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>+0.83%</t>
+          <t>+1.48%</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+14.81%</t>
+          <t>+26.05%</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>2.717</v>
+        <v>4.431</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -716,24 +716,24 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.0592%</t>
+          <t>0.0986%</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>4.7596%</t>
+          <t>5.1597%</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N4" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -742,7 +742,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -764,26 +764,26 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>¥1,001,422.09</t>
+          <t>¥1,003,464.49</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>¥+1,422.09</t>
+          <t>¥+3,464.49</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>+0.14%</t>
+          <t>+0.35%</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+2.42%</t>
+          <t>+5.60%</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>0.252</v>
+        <v>1.575</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -792,24 +792,24 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.0103%</t>
+          <t>0.0232%</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2.4092%</t>
+          <t>2.4506%</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -818,7 +818,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -840,26 +840,26 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>¥1,000,348.00</t>
+          <t>¥1,001,518.00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>¥+348.00</t>
+          <t>¥+1,518.00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>+0.03%</t>
+          <t>+0.15%</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+0.59%</t>
+          <t>+2.42%</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>-1.15</v>
+        <v>0.472</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -868,24 +868,24 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0.0025%</t>
+          <t>0.0101%</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>1.1717%</t>
+          <t>1.2193%</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N6" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -894,7 +894,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -916,26 +916,26 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>¥1,035,947.04</t>
+          <t>¥1,040,563.19</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>¥+35,947.04</t>
+          <t>¥+40,563.19</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>+3.59%</t>
+          <t>+4.06%</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>+81.00%</t>
+          <t>+87.06%</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>7.658</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -944,24 +944,24 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>64.3%</t>
+          <t>66.7%</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>0.2539%</t>
+          <t>0.2667%</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>8.0954%</t>
+          <t>7.8577%</t>
         </is>
       </c>
       <c r="M7" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N7" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -970,7 +970,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -992,26 +992,26 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>¥1,022,227.05</t>
+          <t>¥1,026,881.61</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>¥+22,227.05</t>
+          <t>¥+26,881.61</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>+2.22%</t>
+          <t>+2.69%</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>+44.68%</t>
+          <t>+51.86%</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>5.363</v>
+        <v>6.192</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -1020,24 +1020,24 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>0.1581%</t>
+          <t>0.1779%</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>7.0610%</t>
+          <t>6.9223%</t>
         </is>
       </c>
       <c r="M8" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N8" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -1068,26 +1068,26 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>¥1,024,599.25</t>
+          <t>¥1,030,262.17</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>¥+24,599.25</t>
+          <t>¥+30,262.17</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>+2.46%</t>
+          <t>+3.03%</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>+50.42%</t>
+          <t>+59.93%</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>6</v>
+        <v>6.98</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -1096,24 +1096,24 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>57.1%</t>
+          <t>60.0%</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>0.1747%</t>
+          <t>0.1999%</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>7.0072%</t>
+          <t>6.9331%</t>
         </is>
       </c>
       <c r="M9" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N9" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -1144,26 +1144,26 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>¥1,040,839.33</t>
+          <t>¥1,052,440.53</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>¥+40,839.33</t>
+          <t>¥+52,440.53</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>+4.08%</t>
+          <t>+5.24%</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>+95.91%</t>
+          <t>+123.67%</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>6.271</v>
+        <v>7.436</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -1172,24 +1172,24 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>64.3%</t>
+          <t>66.7%</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>0.2888%</t>
+          <t>0.3439%</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>11.2919%</t>
+          <t>11.3886%</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N10" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1198,7 +1198,7 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -1220,26 +1220,26 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>¥1,001,501.00</t>
+          <t>¥1,002,594.00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>¥+1,501.00</t>
+          <t>¥+2,594.00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>+0.15%</t>
+          <t>+0.26%</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>+2.55%</t>
+          <t>+4.16%</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>0.763</v>
+        <v>2.387</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1248,24 +1248,24 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>0.0107%</t>
+          <t>0.0173%</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>0.9486%</t>
+          <t>0.9959%</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N11" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1274,7 +1274,7 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -1296,26 +1296,26 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>¥1,006,105.34</t>
+          <t>¥1,011,144.42</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>¥+6,105.34</t>
+          <t>¥+11,144.42</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>+0.61%</t>
+          <t>+1.11%</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>+10.77%</t>
+          <t>+19.07%</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>1.94</v>
+        <v>3.44</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1324,24 +1324,24 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>0.0439%</t>
+          <t>0.0744%</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>4.6840%</t>
+          <t>4.8735%</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N12" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -1372,26 +1372,26 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>¥1,033,834.49</t>
+          <t>¥1,042,601.48</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>¥+33,834.49</t>
+          <t>¥+42,601.48</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>+3.38%</t>
+          <t>+4.26%</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>+74.89%</t>
+          <t>+92.91%</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>5.306</v>
+        <v>6.292</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1400,24 +1400,24 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>64.3%</t>
+          <t>66.7%</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>0.2404%</t>
+          <t>0.2809%</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>11.0420%</t>
+          <t>10.9356%</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N13" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -1448,26 +1448,26 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>¥1,005,772.62</t>
+          <t>¥1,007,811.62</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>¥+5,772.62</t>
+          <t>¥+7,811.62</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>+0.58%</t>
+          <t>+0.78%</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>+10.15%</t>
+          <t>+13.04%</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>2.884</v>
+        <v>3.849</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1476,24 +1476,24 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>0.0413%</t>
+          <t>0.0521%</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>2.9213%</t>
+          <t>2.8938%</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N14" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -1524,26 +1524,26 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>¥1,000,131.00</t>
+          <t>¥1,000,596.60</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>¥+131.00</t>
+          <t>¥+596.60</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>+0.01%</t>
+          <t>+0.06%</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>+0.22%</t>
+          <t>+0.94%</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>-3.846</v>
+        <v>-2.063</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1552,24 +1552,24 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>0.0009%</t>
+          <t>0.0040%</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>0.4533%</t>
+          <t>0.4737%</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N15" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -1600,26 +1600,26 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>¥1,000,266.40</t>
+          <t>¥1,000,663.50</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>¥+266.40</t>
+          <t>¥+663.50</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>+0.03%</t>
+          <t>+0.07%</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>+0.45%</t>
+          <t>+1.05%</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>-3.212</v>
+        <v>-1.82</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1628,24 +1628,24 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>0.0019%</t>
+          <t>0.0044%</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>0.4669%</t>
+          <t>0.4752%</t>
         </is>
       </c>
       <c r="M16" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N16" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1654,7 +1654,7 @@
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -1777,26 +1777,26 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>¥1,012,068.30</t>
+          <t>¥1,019,638.10</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>¥+12,068.30</t>
+          <t>¥+19,638.10</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>+1.21%</t>
+          <t>+1.96%</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+22.33%</t>
+          <t>+35.84%</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>3.13</v>
+        <v>4.648</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -1805,24 +1805,24 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>71.4%</t>
+          <t>73.3%</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.0865%</t>
+          <t>0.1306%</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>6.3329%</t>
+          <t>6.6552%</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -1853,26 +1853,26 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>¥1,034,427.67</t>
+          <t>¥1,042,439.98</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>¥+34,427.67</t>
+          <t>¥+42,439.98</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>+3.44%</t>
+          <t>+4.24%</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+76.59%</t>
+          <t>+92.44%</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>5.698</v>
+        <v>6.638</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -1881,24 +1881,24 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>64.3%</t>
+          <t>66.7%</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.2442%</t>
+          <t>0.2796%</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>10.4544%</t>
+          <t>10.3159%</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -1929,26 +1929,26 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>¥1,008,252.47</t>
+          <t>¥1,014,809.18</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>¥+8,252.47</t>
+          <t>¥+14,809.18</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>+0.83%</t>
+          <t>+1.48%</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+14.81%</t>
+          <t>+26.05%</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>2.717</v>
+        <v>4.431</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -1957,24 +1957,24 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.0592%</t>
+          <t>0.0986%</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>4.7596%</t>
+          <t>5.1597%</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N4" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -1983,7 +1983,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -2005,26 +2005,26 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>¥1,001,422.09</t>
+          <t>¥1,003,464.49</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>¥+1,422.09</t>
+          <t>¥+3,464.49</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>+0.14%</t>
+          <t>+0.35%</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+2.42%</t>
+          <t>+5.60%</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>0.252</v>
+        <v>1.575</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -2033,24 +2033,24 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.0103%</t>
+          <t>0.0232%</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>2.4092%</t>
+          <t>2.4506%</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -2059,7 +2059,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -2081,26 +2081,26 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>¥1,000,348.00</t>
+          <t>¥1,001,518.00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>¥+348.00</t>
+          <t>¥+1,518.00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>+0.03%</t>
+          <t>+0.15%</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+0.59%</t>
+          <t>+2.42%</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>-1.15</v>
+        <v>0.472</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -2109,24 +2109,24 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0.0025%</t>
+          <t>0.0101%</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>1.1717%</t>
+          <t>1.2193%</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N6" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -2135,7 +2135,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -2258,26 +2258,26 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>¥1,035,947.04</t>
+          <t>¥1,040,563.19</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>¥+35,947.04</t>
+          <t>¥+40,563.19</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>+3.59%</t>
+          <t>+4.06%</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+81.00%</t>
+          <t>+87.06%</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>7.658</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -2286,24 +2286,24 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>64.3%</t>
+          <t>66.7%</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.2539%</t>
+          <t>0.2667%</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>8.0954%</t>
+          <t>7.8577%</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -2312,7 +2312,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -2334,26 +2334,26 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>¥1,022,227.05</t>
+          <t>¥1,026,881.61</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>¥+22,227.05</t>
+          <t>¥+26,881.61</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>+2.22%</t>
+          <t>+2.69%</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+44.68%</t>
+          <t>+51.86%</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>5.363</v>
+        <v>6.192</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -2362,24 +2362,24 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.1581%</t>
+          <t>0.1779%</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>7.0610%</t>
+          <t>6.9223%</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -2388,7 +2388,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -2410,26 +2410,26 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>¥1,024,599.25</t>
+          <t>¥1,030,262.17</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>¥+24,599.25</t>
+          <t>¥+30,262.17</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>+2.46%</t>
+          <t>+3.03%</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+50.42%</t>
+          <t>+59.93%</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>6</v>
+        <v>6.98</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -2438,24 +2438,24 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>57.1%</t>
+          <t>60.0%</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.1747%</t>
+          <t>0.1999%</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>7.0072%</t>
+          <t>6.9331%</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N4" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -2464,7 +2464,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -2486,26 +2486,26 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>¥1,040,839.33</t>
+          <t>¥1,052,440.53</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>¥+40,839.33</t>
+          <t>¥+52,440.53</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>+4.08%</t>
+          <t>+5.24%</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+95.91%</t>
+          <t>+123.67%</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>6.271</v>
+        <v>7.436</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -2514,24 +2514,24 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>64.3%</t>
+          <t>66.7%</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.2888%</t>
+          <t>0.3439%</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>11.2919%</t>
+          <t>11.3886%</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -2540,7 +2540,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -2562,26 +2562,26 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>¥1,001,501.00</t>
+          <t>¥1,002,594.00</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>¥+1,501.00</t>
+          <t>¥+2,594.00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>+0.15%</t>
+          <t>+0.26%</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+2.55%</t>
+          <t>+4.16%</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>0.763</v>
+        <v>2.387</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -2590,24 +2590,24 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0.0107%</t>
+          <t>0.0173%</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>0.9486%</t>
+          <t>0.9959%</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N6" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -2616,7 +2616,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -2739,26 +2739,26 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>¥1,006,105.34</t>
+          <t>¥1,011,144.42</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>¥+6,105.34</t>
+          <t>¥+11,144.42</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>+0.61%</t>
+          <t>+1.11%</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+10.77%</t>
+          <t>+19.07%</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>1.94</v>
+        <v>3.44</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -2767,24 +2767,24 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.0439%</t>
+          <t>0.0744%</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>4.6840%</t>
+          <t>4.8735%</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N2" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -2793,7 +2793,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -2815,26 +2815,26 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>¥1,033,834.49</t>
+          <t>¥1,042,601.48</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>¥+33,834.49</t>
+          <t>¥+42,601.48</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>+3.38%</t>
+          <t>+4.26%</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+74.89%</t>
+          <t>+92.91%</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>5.306</v>
+        <v>6.292</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -2843,24 +2843,24 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>64.3%</t>
+          <t>66.7%</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>0.2404%</t>
+          <t>0.2809%</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>11.0420%</t>
+          <t>10.9356%</t>
         </is>
       </c>
       <c r="M3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N3" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -2891,26 +2891,26 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>¥1,005,772.62</t>
+          <t>¥1,007,811.62</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>¥+5,772.62</t>
+          <t>¥+7,811.62</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>+0.58%</t>
+          <t>+0.78%</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+10.15%</t>
+          <t>+13.04%</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>2.884</v>
+        <v>3.849</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -2919,24 +2919,24 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>0.0413%</t>
+          <t>0.0521%</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>2.9213%</t>
+          <t>2.8938%</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N4" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -2945,7 +2945,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -2967,26 +2967,26 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>¥1,000,131.00</t>
+          <t>¥1,000,596.60</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>¥+131.00</t>
+          <t>¥+596.60</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>+0.01%</t>
+          <t>+0.06%</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+0.22%</t>
+          <t>+0.94%</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>-3.846</v>
+        <v>-2.063</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -2995,24 +2995,24 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.0009%</t>
+          <t>0.0040%</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>0.4533%</t>
+          <t>0.4737%</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N5" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>
@@ -3043,26 +3043,26 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>¥1,000,266.40</t>
+          <t>¥1,000,663.50</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>¥+266.40</t>
+          <t>¥+663.50</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>+0.03%</t>
+          <t>+0.07%</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+0.45%</t>
+          <t>+1.05%</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>-3.212</v>
+        <v>-1.82</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -3071,24 +3071,24 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>53.3%</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>0.0019%</t>
+          <t>0.0044%</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>0.4669%</t>
+          <t>0.4752%</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N6" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>20260108</t>
+          <t>20260109</t>
         </is>
       </c>
     </row>

</xml_diff>